<commit_message>
updated base class mechanism
</commit_message>
<xml_diff>
--- a/testdata/Opencart_LoginData.xlsx
+++ b/testdata/Opencart_LoginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenCartHybridFramework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D0D5E4-8E62-4B43-B0C5-6D12589AABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42791DA1-AE40-4E90-9BB7-04B8F866D1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -76,12 +76,25 @@
   </si>
   <si>
     <t>abc123@gmail.com</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -151,12 +164,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +192,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,20 +512,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.21875"/>
+    <col min="2" max="2" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" customWidth="true" width="18.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +535,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -519,8 +549,11 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s" s="0">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -530,8 +563,11 @@
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s" s="0">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,8 +577,11 @@
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s" s="0">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -550,10 +589,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -562,6 +604,9 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>